<commit_message>
updated template khd wild vouchers, JSON
</commit_message>
<xml_diff>
--- a/assets/resources/TEMPLATE_DataFields_Vouchers_BioAssets_Wild.xlsx
+++ b/assets/resources/TEMPLATE_DataFields_Vouchers_BioAssets_Wild.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dbotanicgardens.sharepoint.com/sites/FieldWork/Shared Documents/General/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard.levy\.ssh\interactiveGuide\assets\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{FD65F087-051D-4096-B5EA-D1AAEB85768B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{87059924-526D-4415-9195-585C613062FB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B6E70F-6A90-4F99-A184-46C4BEE6E50F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1800" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -300,9 +300,6 @@
     <t>dynamicProperties</t>
   </si>
   <si>
-    <t>format = {"trait":"value"} , {"trait":numericValue} example = {"flowerColor":"purple"} , {"heightInCentimeters":14.3}</t>
-  </si>
-  <si>
     <t>Phenology: flower and fruit; flower; fruit; seed cone; pollen cone; pollen and seed cone; spore; vegetative; reproductive bud; flower and bud; vegetative bud</t>
   </si>
   <si>
@@ -319,6 +316,9 @@
   </si>
   <si>
     <t>iNaturalist ID</t>
+  </si>
+  <si>
+    <t>format = {"trait":"value","trait":numericValue} example = {"flowerColor":"purple","heightInCentimeters":14.3}</t>
   </si>
 </sst>
 </file>
@@ -667,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AW2" sqref="AW2"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,7 +784,7 @@
         <v>16</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="U1" s="2" t="s">
         <v>90</v>
@@ -871,7 +871,7 @@
         <v>68</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AX1" s="1" t="s">
         <v>24</v>
@@ -894,7 +894,7 @@
     </row>
     <row r="2" spans="1:55" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>67</v>
@@ -939,13 +939,13 @@
         <v>23</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="U2" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="V2" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="V2" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="W2" s="4" t="s">
         <v>57</v>
@@ -1020,7 +1020,7 @@
         <v>61</v>
       </c>
       <c r="AZ2" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BA2" s="4" t="s">
         <v>34</v>
@@ -1036,21 +1036,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D1BE5CD796B69543BA7FCF39B9A430F9" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="48f98be3a9b998f19577fe96e9026a80">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf26cdc5-6581-43e5-a643-41a56d0810f3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="73b90b828ce3bab7196225ca911adf86" ns2:_="">
     <xsd:import namespace="bf26cdc5-6581-43e5-a643-41a56d0810f3"/>
@@ -1234,11 +1219,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A5FA02A-BE01-4CF0-9B30-F8CA8555C0C6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8CCA6BC-CC7C-42F3-8E95-F6068EA83625}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bf26cdc5-6581-43e5-a643-41a56d0810f3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1252,5 +1261,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8CCA6BC-CC7C-42F3-8E95-F6068EA83625}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A5FA02A-BE01-4CF0-9B30-F8CA8555C0C6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>